<commit_message>
Complete update. all numeric inputs. header and two column output.
</commit_message>
<xml_diff>
--- a/src/assets/FC Tree Pulling Database Variables versus ForestGALES Java Code Variables.xlsx
+++ b/src/assets/FC Tree Pulling Database Variables versus ForestGALES Java Code Variables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
   <si>
     <t>Tree Pulling Database Parameter</t>
   </si>
@@ -242,9 +242,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>String (text) - supplied in code as 'Gley'</t>
-  </si>
-  <si>
     <t>ignored</t>
   </si>
   <si>
@@ -386,6 +383,30 @@
       </rPr>
       <t>HeightOfForce = 0</t>
     </r>
+  </si>
+  <si>
+    <t>dams</t>
+  </si>
+  <si>
+    <t>topHeight</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>drainage</t>
+  </si>
+  <si>
+    <t>cultivation</t>
+  </si>
+  <si>
+    <t>brownEdge</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -473,15 +494,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -504,13 +537,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -523,12 +581,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -846,7 +929,7 @@
     <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
     <col min="6" max="6" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -877,7 +960,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -895,7 +978,7 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -904,7 +987,7 @@
       <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>54</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -912,23 +995,23 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+    <row r="5" spans="1:6" s="12" customFormat="1">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
@@ -951,7 +1034,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -961,7 +1044,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>47</v>
@@ -1015,13 +1098,13 @@
         <v>28</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
+      <c r="A11" s="11">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1049,7 +1132,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>47</v>
@@ -1067,7 +1150,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>47</v>
@@ -1085,7 +1168,7 @@
         <v>38</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>47</v>
@@ -1103,7 +1186,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>47</v>
@@ -1121,7 +1204,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>47</v>
@@ -1129,7 +1212,7 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17">
+      <c r="A17" s="11">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1139,7 +1222,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>47</v>
@@ -1157,7 +1240,7 @@
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>47</v>
@@ -1175,7 +1258,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
@@ -1191,7 +1274,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>30</v>
@@ -1211,7 +1294,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>30</v>
@@ -1229,13 +1312,13 @@
         <v>44</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23">
+      <c r="A23" s="11">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1245,7 +1328,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>47</v>
@@ -1263,12 +1346,97 @@
         <v>46</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" s="12" customFormat="1">
+      <c r="A25" s="11">
+        <v>23</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="12" customFormat="1">
+      <c r="A26" s="11">
+        <v>24</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="12" customFormat="1">
+      <c r="A27" s="11">
+        <v>25</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="12" customFormat="1">
+      <c r="A28" s="11">
+        <v>26</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="12" customFormat="1">
+      <c r="A29" s="11">
+        <v>27</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>